<commit_message>
update sheets so for proper data entry
</commit_message>
<xml_diff>
--- a/py/app/data/raw_scouting_data.xlsx
+++ b/py/app/data/raw_scouting_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ScoutingInfo" sheetId="1" state="visible" r:id="rId1"/>
@@ -482,7 +482,7 @@
   </sheetPr>
   <dimension ref="A1:Y343"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="A2:Y999"/>
     </sheetView>
   </sheetViews>
@@ -32411,7 +32411,7 @@
   </sheetPr>
   <dimension ref="A1:AB500"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q14" sqref="A2:AB500"/>
     </sheetView>
   </sheetViews>

</xml_diff>